<commit_message>
Corrected a fairly large mistake
</commit_message>
<xml_diff>
--- a/data/clean_worksheet.xlsx
+++ b/data/clean_worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Home\DasCrazy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC37991-73A0-4F15-9C94-789559CCD32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967C1942-1B4C-4E5A-9589-2EC0CF2927A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16220" yWindow="5830" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="4470" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clean_condensed" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -47,13 +47,19 @@
   <si>
     <t>moment_rate</t>
   </si>
+  <si>
+    <t>Nailogical stream; includes parts of day 7/6</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -535,7 +541,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -891,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,9 +908,10 @@
     <col min="1" max="1" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -917,23 +924,26 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>44366</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>35599</v>
       </c>
       <c r="D2" s="2">
-        <f>B2/C2</f>
-        <v>7.0226691761004524E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" ref="D2:D27" si="0">B2/C2</f>
+        <v>5.8990421079243801E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>44368</v>
       </c>
@@ -944,146 +954,146 @@
         <v>36118</v>
       </c>
       <c r="D3" s="2">
-        <f>B3/C3</f>
+        <f t="shared" si="0"/>
         <v>6.0911456891300732E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>44369</v>
       </c>
       <c r="B4">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>39282</v>
       </c>
       <c r="D4" s="2">
-        <f>B4/C4</f>
-        <v>9.1645028257217049E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>7.891655211038134E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44370</v>
       </c>
       <c r="B5">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>33432</v>
       </c>
       <c r="D5" s="2">
-        <f>B5/C5</f>
-        <v>1.6152189519023691E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.4656616415410384E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44371</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>27843</v>
       </c>
       <c r="D6" s="2">
-        <f>B6/C6</f>
-        <v>6.1056639011600764E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>5.7465072010918366E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44372</v>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C7">
         <v>34758</v>
       </c>
       <c r="D7" s="2">
-        <f>B7/C7</f>
-        <v>7.1925887565452552E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>5.7540710052362046E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44373</v>
       </c>
       <c r="B8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>32308</v>
       </c>
       <c r="D8" s="2">
-        <f>B8/C8</f>
-        <v>4.9523337872972638E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>4.6428129255911846E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44375</v>
       </c>
       <c r="B9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>24026</v>
       </c>
       <c r="D9" s="2">
-        <f>B9/C9</f>
-        <v>9.5729626238241902E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>9.1567468575709651E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44376</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>27352</v>
       </c>
       <c r="D10" s="2">
-        <f>B10/C10</f>
-        <v>1.0968119333138345E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>9.1400994442819539E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44378</v>
       </c>
       <c r="B11">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>31382</v>
       </c>
       <c r="D11" s="2">
-        <f>B11/C11</f>
-        <v>7.9663501370212219E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>7.647696131540373E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44379</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12">
         <v>26874</v>
       </c>
       <c r="D12" s="2">
-        <f>B12/C12</f>
-        <v>1.1163206072784104E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>1.0046885465505692E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44380</v>
       </c>
@@ -1094,26 +1104,26 @@
         <v>27970</v>
       </c>
       <c r="D13" s="2">
-        <f>B13/C13</f>
+        <f t="shared" si="0"/>
         <v>4.2903110475509475E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44381</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14">
         <v>12198</v>
       </c>
       <c r="D14" s="2">
-        <f>B14/C14</f>
-        <v>6.5584522052795544E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>5.7386456796196098E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44382</v>
       </c>
@@ -1124,23 +1134,26 @@
         <v>37674</v>
       </c>
       <c r="D15" s="2">
-        <f>B15/C15</f>
+        <f t="shared" si="0"/>
         <v>9.8210967776185174E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>44383</v>
       </c>
       <c r="B16">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>23828</v>
       </c>
       <c r="D16" s="2">
-        <f>B16/C16</f>
-        <v>9.2328353197918412E-4</v>
+        <f t="shared" si="0"/>
+        <v>7.1344636562027869E-4</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -1148,14 +1161,14 @@
         <v>44384</v>
       </c>
       <c r="B17">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>30964</v>
       </c>
       <c r="D17" s="2">
-        <f>B17/C17</f>
-        <v>8.3968479524609222E-4</v>
+        <f t="shared" si="0"/>
+        <v>7.7509365715023898E-4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -1163,14 +1176,14 @@
         <v>44385</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>29289</v>
       </c>
       <c r="D18" s="2">
-        <f>B18/C18</f>
-        <v>5.4628017344395506E-4</v>
+        <f t="shared" si="0"/>
+        <v>5.1213766260370787E-4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1184,7 +1197,7 @@
         <v>29136</v>
       </c>
       <c r="D19" s="2">
-        <f>B19/C19</f>
+        <f t="shared" si="0"/>
         <v>7.5507962657880281E-4</v>
       </c>
     </row>
@@ -1193,14 +1206,14 @@
         <v>44387</v>
       </c>
       <c r="B20">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20">
         <v>38334</v>
       </c>
       <c r="D20" s="2">
-        <f>B20/C20</f>
-        <v>7.5650858245943553E-4</v>
+        <f t="shared" si="0"/>
+        <v>7.3042207961600671E-4</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1208,14 +1221,14 @@
         <v>44388</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21">
         <v>27061</v>
       </c>
       <c r="D21" s="2">
-        <f>B21/C21</f>
-        <v>7.021174383799564E-4</v>
+        <f t="shared" si="0"/>
+        <v>6.2821033960311888E-4</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -1223,14 +1236,14 @@
         <v>44389</v>
       </c>
       <c r="B22">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>35765</v>
       </c>
       <c r="D22" s="2">
-        <f>B22/C22</f>
-        <v>1.3420942261987978E-3</v>
+        <f t="shared" si="0"/>
+        <v>1.1463721515448063E-3</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -1238,14 +1251,14 @@
         <v>44390</v>
       </c>
       <c r="B23">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>30202</v>
       </c>
       <c r="D23" s="2">
-        <f>B23/C23</f>
-        <v>1.1588636514138137E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.2709092113105087E-4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -1253,14 +1266,14 @@
         <v>44391</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>27916</v>
       </c>
       <c r="D24" s="2">
-        <f>B24/C24</f>
-        <v>1.0746525290156184E-3</v>
+        <f t="shared" si="0"/>
+        <v>9.3136552514686921E-4</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -1268,14 +1281,14 @@
         <v>44392</v>
       </c>
       <c r="B25">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C25">
         <v>23523</v>
       </c>
       <c r="D25" s="2">
-        <f>B25/C25</f>
-        <v>8.9274327254176768E-4</v>
+        <f t="shared" si="0"/>
+        <v>8.0772010372826594E-4</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -1283,14 +1296,14 @@
         <v>44393</v>
       </c>
       <c r="B26">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>28716</v>
       </c>
       <c r="D26" s="2">
-        <f>B26/C26</f>
-        <v>7.6612341551748149E-4</v>
+        <f t="shared" si="0"/>
+        <v>7.3129962390305057E-4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -1298,14 +1311,14 @@
         <v>44394</v>
       </c>
       <c r="B27">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>26186</v>
       </c>
       <c r="D27" s="2">
-        <f>B27/C27</f>
-        <v>8.4014358817688839E-4</v>
+        <f t="shared" si="0"/>
+        <v>8.0195524325975709E-4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -1317,7 +1330,7 @@
       </c>
       <c r="D29" s="2">
         <f>AVERAGE(D2:D27)</f>
-        <v>8.5768207754505145E-4</v>
+        <v>7.7355871137680711E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>